<commit_message>
Added some helper functions
</commit_message>
<xml_diff>
--- a/Queenstown.xlsx
+++ b/Queenstown.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -937,6 +937,454 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Queenstown</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>05-23</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>RWE</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>RWE</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>RWE 1</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Queenstown</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>05-23</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>RWE</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>RWE</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>RWE 2</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Queenstown</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>05-23</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>RWE</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>RWE</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>RWE 3</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Queenstown</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>05-23</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>RCL</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>RCL</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>RCL 1</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Queenstown</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>05-23</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>RCL</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>RCL</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>RCL 2</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Queenstown</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>05-23</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>RCL</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>RCL</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>RCL 3</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Queenstown</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>05-23</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>TWY</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>TWY</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>TWY</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>